<commit_message>
fixed error in graph
</commit_message>
<xml_diff>
--- a/editedresults.xlsx
+++ b/editedresults.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A3354B71-5091-4D93-B1DD-0278E9059F02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD52FEF7-39D3-4CA5-BC9E-D48912BE562E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="editedresults" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8618,6 +8618,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>editedresults!$AF$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -8644,10 +8655,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>editedresults!$AF$2:$AF$12</c:f>
+              <c:f>editedresults!$AF$2:$AF$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10.591333329999999</c:v>
                 </c:pt>
@@ -8677,9 +8688,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>6.0720000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.5473333330000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11880,11 +11888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>